<commit_message>
added chart for Question 6
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\NSS\DA9\Excel\lookups_exercise-robintietz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309E1FEC-53F0-459F-8872-33F82F3C87A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B96BA8D-B92B-4A06-AC5B-F2CBB68B8454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -901,6 +901,974 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20862700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22683800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23220300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1B77-4023-A226-F7E2830FBFF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20036743.4099999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21722126.219999898</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22619057.440000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1B77-4023-A226-F7E2830FBFF3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="551710296"/>
+        <c:axId val="551712096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="551710296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551712096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="551712096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="551710296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A99AFB0-E7F6-1D7A-BB74-3FA00E94588C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1200,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,7 +2314,7 @@
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">_xlfn.RANK.EQ(E3,E$2:E$52,1)</f>
+        <f>_xlfn.RANK.EQ(E3,E$2:E$52,1)</f>
         <v>22</v>
       </c>
       <c r="G3">
@@ -1356,15 +2324,15 @@
         <v>312433.70999999897</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I52" si="3">H3-G3</f>
+        <f t="shared" ref="I3:I52" si="2">H3-G3</f>
         <v>-22366.290000001027</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3:J52" si="4">IF(I3=0,"",I3/G3)</f>
+        <f t="shared" ref="J3:J52" si="3">IF(I3=0,"",I3/G3)</f>
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">_xlfn.RANK.EQ(J3,J$2:J$52,1)</f>
+        <f t="shared" ref="K3:K52" si="4">_xlfn.RANK.EQ(J3,J$2:J$52,1)</f>
         <v>14</v>
       </c>
       <c r="L3">
@@ -1374,15 +2342,15 @@
         <v>322263.03999999998</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N52" si="6">M3-L3</f>
+        <f t="shared" ref="N3:N52" si="5">M3-L3</f>
         <v>-436.96000000002095</v>
       </c>
       <c r="O3" s="5">
-        <f t="shared" ref="O3:O52" si="7">IF(N3=0,"",N3/L3)</f>
+        <f t="shared" ref="O3:O52" si="6">IF(N3=0,"",N3/L3)</f>
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">_xlfn.RANK.EQ(O3,O$2:O$52,1)</f>
+        <f t="shared" ref="P3:P52" si="7">_xlfn.RANK.EQ(O3,O$2:O$52,1)</f>
         <v>37</v>
       </c>
     </row>
@@ -1405,7 +2373,7 @@
         <v>-4.9327413275443007E-3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F3:F52" si="8">_xlfn.RANK.EQ(E4,E$2:E$52,1)</f>
         <v>42</v>
       </c>
       <c r="G4">
@@ -1415,15 +2383,15 @@
         <v>3589693.2099999902</v>
       </c>
       <c r="I4">
+        <f t="shared" si="2"/>
+        <v>-62606.790000009816</v>
+      </c>
+      <c r="J4" s="5">
         <f t="shared" si="3"/>
-        <v>-62606.790000009816</v>
-      </c>
-      <c r="J4" s="5">
+        <v>-1.7141743558856015E-2</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="4"/>
-        <v>-1.7141743558856015E-2</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="L4">
@@ -1433,15 +2401,15 @@
         <v>3564983.04999999</v>
       </c>
       <c r="N4">
+        <f t="shared" si="5"/>
+        <v>-97416.950000009965</v>
+      </c>
+      <c r="O4" s="5">
         <f t="shared" si="6"/>
-        <v>-97416.950000009965</v>
-      </c>
-      <c r="O4" s="5">
+        <v>-2.6599210899959033E-2</v>
+      </c>
+      <c r="P4">
         <f t="shared" si="7"/>
-        <v>-2.6599210899959033E-2</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="8"/>
         <v>25</v>
       </c>
     </row>
@@ -1464,7 +2432,7 @@
         <v>-9.4273968477453174E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="G5">
@@ -1474,15 +2442,15 @@
         <v>7020609.3200000003</v>
       </c>
       <c r="I5">
+        <f t="shared" si="2"/>
+        <v>-947690.6799999997</v>
+      </c>
+      <c r="J5" s="5">
         <f t="shared" si="3"/>
-        <v>-947690.6799999997</v>
-      </c>
-      <c r="J5" s="5">
+        <v>-0.118932605449092</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="4"/>
-        <v>-0.118932605449092</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="L5">
@@ -1492,15 +2460,15 @@
         <v>7497322.9100000001</v>
       </c>
       <c r="N5">
+        <f t="shared" si="5"/>
+        <v>-262277.08999999985</v>
+      </c>
+      <c r="O5" s="5">
         <f t="shared" si="6"/>
-        <v>-262277.08999999985</v>
-      </c>
-      <c r="O5" s="5">
+        <v>-3.3800336357544182E-2</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="7"/>
-        <v>-3.3800336357544182E-2</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="8"/>
         <v>22</v>
       </c>
     </row>
@@ -1523,7 +2491,7 @@
         <v>-5.7149963352064452E-2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="G6">
@@ -1533,15 +2501,15 @@
         <v>427758.64</v>
       </c>
       <c r="I6">
+        <f t="shared" si="2"/>
+        <v>-741.35999999998603</v>
+      </c>
+      <c r="J6" s="5">
         <f t="shared" si="3"/>
-        <v>-741.35999999998603</v>
-      </c>
-      <c r="J6" s="5">
+        <v>-1.7301283547257551E-3</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="4"/>
-        <v>-1.7301283547257551E-3</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="L6">
@@ -1551,15 +2519,15 @@
         <v>445114.28999999899</v>
       </c>
       <c r="N6">
+        <f t="shared" si="5"/>
+        <v>-85.710000001010485</v>
+      </c>
+      <c r="O6" s="5">
         <f t="shared" si="6"/>
-        <v>-85.710000001010485</v>
-      </c>
-      <c r="O6" s="5">
+        <v>-1.925202156356929E-4</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="7"/>
-        <v>-1.925202156356929E-4</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="8"/>
         <v>39</v>
       </c>
     </row>
@@ -1582,7 +2550,7 @@
         <v>-0.11502817362571344</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="G7">
@@ -1592,15 +2560,15 @@
         <v>3051483.41</v>
       </c>
       <c r="I7">
+        <f t="shared" si="2"/>
+        <v>-339416.58999999985</v>
+      </c>
+      <c r="J7" s="5">
         <f t="shared" si="3"/>
-        <v>-339416.58999999985</v>
-      </c>
-      <c r="J7" s="5">
+        <v>-0.10009631366303927</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="4"/>
-        <v>-0.10009631366303927</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="L7">
@@ -1610,15 +2578,15 @@
         <v>2946440.08</v>
       </c>
       <c r="N7">
+        <f t="shared" si="5"/>
+        <v>-398759.91999999993</v>
+      </c>
+      <c r="O7" s="5">
         <f t="shared" si="6"/>
-        <v>-398759.91999999993</v>
-      </c>
-      <c r="O7" s="5">
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="7"/>
-        <v>-0.11920361114432618</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="8"/>
         <v>4</v>
       </c>
     </row>
@@ -1641,7 +2609,7 @@
         <v>-0.15235918433091292</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="G8">
@@ -1651,15 +2619,15 @@
         <v>1383905.98999999</v>
       </c>
       <c r="I8">
+        <f t="shared" si="2"/>
+        <v>-206794.01000001002</v>
+      </c>
+      <c r="J8" s="5">
         <f t="shared" si="3"/>
-        <v>-206794.01000001002</v>
-      </c>
-      <c r="J8" s="5">
+        <v>-0.13000189224870184</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="4"/>
-        <v>-0.13000189224870184</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="L8">
@@ -1669,15 +2637,15 @@
         <v>1337735.3199999901</v>
       </c>
       <c r="N8">
+        <f t="shared" si="5"/>
+        <v>-241564.68000000995</v>
+      </c>
+      <c r="O8" s="5">
         <f t="shared" si="6"/>
-        <v>-241564.68000000995</v>
-      </c>
-      <c r="O8" s="5">
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="7"/>
-        <v>-0.15295680364719175</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="8"/>
         <v>2</v>
       </c>
     </row>
@@ -1700,7 +2668,7 @@
         <v>-4.2417130511048909E-2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="G9">
@@ -1710,15 +2678,15 @@
         <v>9929059.5199999996</v>
       </c>
       <c r="I9">
+        <f t="shared" si="2"/>
+        <v>-1144640.4800000004</v>
+      </c>
+      <c r="J9" s="5">
         <f t="shared" si="3"/>
-        <v>-1144640.4800000004</v>
-      </c>
-      <c r="J9" s="5">
+        <v>-0.10336567542917005</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="4"/>
-        <v>-0.10336567542917005</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="5"/>
         <v>7</v>
       </c>
       <c r="L9">
@@ -1728,15 +2696,15 @@
         <v>9993599.52999999</v>
       </c>
       <c r="N9">
+        <f t="shared" si="5"/>
+        <v>-796900.47000000998</v>
+      </c>
+      <c r="O9" s="5">
         <f t="shared" si="6"/>
-        <v>-796900.47000000998</v>
-      </c>
-      <c r="O9" s="5">
+        <v>-7.3852043000788653E-2</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="7"/>
-        <v>-7.3852043000788653E-2</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="8"/>
         <v>9</v>
       </c>
     </row>
@@ -1759,7 +2727,7 @@
         <v>-8.1681998646514792E-2</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6</v>
       </c>
       <c r="G10">
@@ -1769,15 +2737,15 @@
         <v>467907.84000000003</v>
       </c>
       <c r="I10">
+        <f t="shared" si="2"/>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="J10" s="5">
         <f t="shared" si="3"/>
-        <v>-27292.159999999974</v>
-      </c>
-      <c r="J10" s="5">
+        <v>-5.5113408723747932E-2</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="4"/>
-        <v>-5.5113408723747932E-2</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="L10">
@@ -1787,15 +2755,15 @@
         <v>478318.92</v>
       </c>
       <c r="N10">
+        <f t="shared" si="5"/>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="O10" s="5">
         <f t="shared" si="6"/>
-        <v>-9181.0800000000163</v>
-      </c>
-      <c r="O10" s="5">
+        <v>-1.883298461538465E-2</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="7"/>
-        <v>-1.883298461538465E-2</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="8"/>
         <v>29</v>
       </c>
     </row>
@@ -1818,7 +2786,7 @@
         <v/>
       </c>
       <c r="F11" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G11">
@@ -1828,15 +2796,15 @@
         <v>0</v>
       </c>
       <c r="I11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="e">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K11" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="L11">
@@ -1846,7 +2814,7 @@
         <v>63771.91</v>
       </c>
       <c r="N11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-311228.08999999997</v>
       </c>
       <c r="O11" s="5">
@@ -1854,7 +2822,7 @@
         <v>-0.82994157333333329</v>
       </c>
       <c r="P11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -1877,7 +2845,7 @@
         <v>-5.0060657805601608E-2</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="G12">
@@ -1887,15 +2855,15 @@
         <v>4205555.5999999996</v>
       </c>
       <c r="I12">
+        <f t="shared" si="2"/>
+        <v>-494844.40000000037</v>
+      </c>
+      <c r="J12" s="5">
         <f t="shared" si="3"/>
-        <v>-494844.40000000037</v>
-      </c>
-      <c r="J12" s="5">
+        <v>-0.10527708280146378</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="4"/>
-        <v>-0.10527708280146378</v>
-      </c>
-      <c r="K12">
-        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="L12">
@@ -1905,15 +2873,15 @@
         <v>4371713.1399999997</v>
       </c>
       <c r="N12">
+        <f t="shared" si="5"/>
+        <v>-306086.86000000034</v>
+      </c>
+      <c r="O12" s="5">
         <f t="shared" si="6"/>
-        <v>-306086.86000000034</v>
-      </c>
-      <c r="O12" s="5">
+        <v>-6.5433934755654441E-2</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="7"/>
-        <v>-6.5433934755654441E-2</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="8"/>
         <v>10</v>
       </c>
     </row>
@@ -1936,7 +2904,7 @@
         <v>-1.2912833886247806E-2</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
       <c r="G13">
@@ -1946,15 +2914,15 @@
         <v>5909077.9399999902</v>
       </c>
       <c r="I13">
+        <f t="shared" si="2"/>
+        <v>-314622.06000000983</v>
+      </c>
+      <c r="J13" s="5">
         <f t="shared" si="3"/>
-        <v>-314622.06000000983</v>
-      </c>
-      <c r="J13" s="5">
+        <v>-5.0552253482656594E-2</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="4"/>
-        <v>-5.0552253482656594E-2</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="L13">
@@ -1964,15 +2932,15 @@
         <v>6056976.6699999999</v>
       </c>
       <c r="N13">
+        <f t="shared" si="5"/>
+        <v>-150323.33000000007</v>
+      </c>
+      <c r="O13" s="5">
         <f t="shared" si="6"/>
-        <v>-150323.33000000007</v>
-      </c>
-      <c r="O13" s="5">
+        <v>-2.4217184605222895E-2</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="7"/>
-        <v>-2.4217184605222895E-2</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="8"/>
         <v>27</v>
       </c>
     </row>
@@ -1995,7 +2963,7 @@
         <v>-1.3637949218750009E-2</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
       <c r="G14">
@@ -2005,15 +2973,15 @@
         <v>524402.98</v>
       </c>
       <c r="I14">
+        <f t="shared" si="2"/>
+        <v>-6097.0200000000186</v>
+      </c>
+      <c r="J14" s="5">
         <f t="shared" si="3"/>
-        <v>-6097.0200000000186</v>
-      </c>
-      <c r="J14" s="5">
+        <v>-1.1492968897266765E-2</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="4"/>
-        <v>-1.1492968897266765E-2</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="5"/>
         <v>40</v>
       </c>
       <c r="L14">
@@ -2023,15 +2991,15 @@
         <v>504989.88</v>
       </c>
       <c r="N14">
+        <f t="shared" si="5"/>
+        <v>-21210.119999999995</v>
+      </c>
+      <c r="O14" s="5">
         <f t="shared" si="6"/>
-        <v>-21210.119999999995</v>
-      </c>
-      <c r="O14" s="5">
+        <v>-4.0308095781071827E-2</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="7"/>
-        <v>-4.0308095781071827E-2</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="8"/>
         <v>19</v>
       </c>
     </row>
@@ -2054,7 +3022,7 @@
         <v>3.1837408866824991E-3</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
       <c r="G15">
@@ -2064,15 +3032,15 @@
         <v>175966389.24999899</v>
       </c>
       <c r="I15">
+        <f t="shared" si="2"/>
+        <v>-8201410.7500010133</v>
+      </c>
+      <c r="J15" s="5">
         <f t="shared" si="3"/>
-        <v>-8201410.7500010133</v>
-      </c>
-      <c r="J15" s="5">
+        <v>-4.4532273014072019E-2</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="4"/>
-        <v>-4.4532273014072019E-2</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="L15">
@@ -2082,15 +3050,15 @@
         <v>184450910.84999901</v>
       </c>
       <c r="N15">
+        <f t="shared" si="5"/>
+        <v>-4502589.1500009894</v>
+      </c>
+      <c r="O15" s="5">
         <f t="shared" si="6"/>
-        <v>-4502589.1500009894</v>
-      </c>
-      <c r="O15" s="5">
+        <v>-2.3829085727446114E-2</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="7"/>
-        <v>-2.3829085727446114E-2</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="8"/>
         <v>28</v>
       </c>
     </row>
@@ -2113,7 +3081,7 @@
         <v>-1.1850188616360429E-2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
       <c r="G16">
@@ -2123,15 +3091,15 @@
         <v>7350464.0800000001</v>
       </c>
       <c r="I16">
+        <f t="shared" si="2"/>
+        <v>-2035.9199999999255</v>
+      </c>
+      <c r="J16" s="5">
         <f t="shared" si="3"/>
-        <v>-2035.9199999999255</v>
-      </c>
-      <c r="J16" s="5">
+        <v>-2.769017341040361E-4</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="4"/>
-        <v>-2.769017341040361E-4</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="5"/>
         <v>46</v>
       </c>
       <c r="L16">
@@ -2141,15 +3109,15 @@
         <v>7397093</v>
       </c>
       <c r="N16">
+        <f t="shared" si="5"/>
+        <v>-107</v>
+      </c>
+      <c r="O16" s="5">
         <f t="shared" si="6"/>
-        <v>-107</v>
-      </c>
-      <c r="O16" s="5">
+        <v>-1.4464932677229222E-5</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="7"/>
-        <v>-1.4464932677229222E-5</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="8"/>
         <v>43</v>
       </c>
     </row>
@@ -2172,7 +3140,7 @@
         <v>-2.8351094826658003E-2</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="G17">
@@ -2182,15 +3150,15 @@
         <v>14645233.51</v>
       </c>
       <c r="I17">
+        <f t="shared" si="2"/>
+        <v>-664466.49000000022</v>
+      </c>
+      <c r="J17" s="5">
         <f t="shared" si="3"/>
-        <v>-664466.49000000022</v>
-      </c>
-      <c r="J17" s="5">
+        <v>-4.3401666263871937E-2</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="4"/>
-        <v>-4.3401666263871937E-2</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="L17">
@@ -2200,15 +3168,15 @@
         <v>14346057.039999999</v>
       </c>
       <c r="N17">
+        <f t="shared" si="5"/>
+        <v>-965742.96000000089</v>
+      </c>
+      <c r="O17" s="5">
         <f t="shared" si="6"/>
-        <v>-965742.96000000089</v>
-      </c>
-      <c r="O17" s="5">
+        <v>-6.3071811282801551E-2</v>
+      </c>
+      <c r="P17">
         <f t="shared" si="7"/>
-        <v>-6.3071811282801551E-2</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="8"/>
         <v>11</v>
       </c>
     </row>
@@ -2231,7 +3199,7 @@
         <v>-5.4037002206391245E-2</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="G18">
@@ -2241,15 +3209,15 @@
         <v>2671745.94</v>
       </c>
       <c r="I18">
+        <f t="shared" si="2"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="J18" s="5">
         <f t="shared" si="3"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="J18" s="5">
+        <v>-6.6149619014330668E-2</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="4"/>
-        <v>-6.6149619014330668E-2</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="5"/>
         <v>15</v>
       </c>
       <c r="L18">
@@ -2259,15 +3227,15 @@
         <v>2535637.09</v>
       </c>
       <c r="N18">
+        <f t="shared" si="5"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="O18" s="5">
         <f t="shared" si="6"/>
-        <v>-374962.91000000015</v>
-      </c>
-      <c r="O18" s="5">
+        <v>-0.12882667147667154</v>
+      </c>
+      <c r="P18">
         <f t="shared" si="7"/>
-        <v>-0.12882667147667154</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="8"/>
         <v>3</v>
       </c>
     </row>
@@ -2290,7 +3258,7 @@
         <v>-4.258504294298146E-2</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="G19">
@@ -2300,15 +3268,15 @@
         <v>8991707.2399999909</v>
       </c>
       <c r="I19">
+        <f t="shared" si="2"/>
+        <v>-721592.76000000909</v>
+      </c>
+      <c r="J19" s="5">
         <f t="shared" si="3"/>
-        <v>-721592.76000000909</v>
-      </c>
-      <c r="J19" s="5">
+        <v>-7.4289145810384635E-2</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="4"/>
-        <v>-7.4289145810384635E-2</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="L19">
@@ -2318,15 +3286,15 @@
         <v>8766655.9100000001</v>
       </c>
       <c r="N19">
+        <f t="shared" si="5"/>
+        <v>-576344.08999999985</v>
+      </c>
+      <c r="O19" s="5">
         <f t="shared" si="6"/>
-        <v>-576344.08999999985</v>
-      </c>
-      <c r="O19" s="5">
+        <v>-6.1687262121374278E-2</v>
+      </c>
+      <c r="P19">
         <f t="shared" si="7"/>
-        <v>-6.1687262121374278E-2</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="8"/>
         <v>12</v>
       </c>
     </row>
@@ -2349,7 +3317,7 @@
         <v>-1.2379538203300809E-5</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>46</v>
       </c>
       <c r="G20">
@@ -2359,15 +3327,15 @@
         <v>131839624.37</v>
       </c>
       <c r="I20">
+        <f t="shared" si="2"/>
+        <v>-9775.6299999952316</v>
+      </c>
+      <c r="J20" s="5">
         <f t="shared" si="3"/>
-        <v>-9775.6299999952316</v>
-      </c>
-      <c r="J20" s="5">
+        <v>-7.4142392760188761E-5</v>
+      </c>
+      <c r="K20">
         <f t="shared" si="4"/>
-        <v>-7.4142392760188761E-5</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="5"/>
         <v>47</v>
       </c>
       <c r="L20">
@@ -2377,15 +3345,15 @@
         <v>130621283.53999899</v>
       </c>
       <c r="N20">
+        <f t="shared" si="5"/>
+        <v>-116.46000100672245</v>
+      </c>
+      <c r="O20" s="5">
         <f t="shared" si="6"/>
-        <v>-116.46000100672245</v>
-      </c>
-      <c r="O20" s="5">
+        <v>-8.9158438821450736E-7</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="7"/>
-        <v>-8.9158438821450736E-7</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="8"/>
         <v>46</v>
       </c>
     </row>
@@ -2408,7 +3376,7 @@
         <v>-7.9052463618023094E-2</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9</v>
       </c>
       <c r="G21">
@@ -2418,15 +3386,15 @@
         <v>22655993.629999999</v>
       </c>
       <c r="I21">
+        <f t="shared" si="2"/>
+        <v>-1841406.370000001</v>
+      </c>
+      <c r="J21" s="5">
         <f t="shared" si="3"/>
-        <v>-1841406.370000001</v>
-      </c>
-      <c r="J21" s="5">
+        <v>-7.5167420624229556E-2</v>
+      </c>
+      <c r="K21">
         <f t="shared" si="4"/>
-        <v>-7.5167420624229556E-2</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="L21">
@@ -2436,15 +3404,15 @@
         <v>23434073.089999899</v>
       </c>
       <c r="N21">
+        <f t="shared" si="5"/>
+        <v>-888926.91000010073</v>
+      </c>
+      <c r="O21" s="5">
         <f t="shared" si="6"/>
-        <v>-888926.91000010073</v>
-      </c>
-      <c r="O21" s="5">
+        <v>-3.6546762734864152E-2</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="7"/>
-        <v>-3.6546762734864152E-2</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="8"/>
         <v>21</v>
       </c>
     </row>
@@ -2467,7 +3435,7 @@
         <v>-1.3285502334437123E-2</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
       <c r="G22">
@@ -2477,15 +3445,15 @@
         <v>11791977.9699999</v>
       </c>
       <c r="I22">
+        <f t="shared" si="2"/>
+        <v>-188722.03000009991</v>
+      </c>
+      <c r="J22" s="5">
         <f t="shared" si="3"/>
-        <v>-188722.03000009991</v>
-      </c>
-      <c r="J22" s="5">
+        <v>-1.5752170574348738E-2</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="4"/>
-        <v>-1.5752170574348738E-2</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="L22">
@@ -2495,15 +3463,15 @@
         <v>11934454.77</v>
       </c>
       <c r="N22">
+        <f t="shared" si="5"/>
+        <v>-745.23000000044703</v>
+      </c>
+      <c r="O22" s="5">
         <f t="shared" si="6"/>
-        <v>-745.23000000044703</v>
-      </c>
-      <c r="O22" s="5">
+        <v>-6.2439674240938325E-5</v>
+      </c>
+      <c r="P22">
         <f t="shared" si="7"/>
-        <v>-6.2439674240938325E-5</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="8"/>
         <v>42</v>
       </c>
     </row>
@@ -2526,7 +3494,7 @@
         <v>-3.9590110100806722E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="G23">
@@ -2536,15 +3504,15 @@
         <v>21722126.219999898</v>
       </c>
       <c r="I23">
+        <f t="shared" si="2"/>
+        <v>-961673.78000010177</v>
+      </c>
+      <c r="J23" s="5">
         <f t="shared" si="3"/>
-        <v>-961673.78000010177</v>
-      </c>
-      <c r="J23" s="5">
+        <v>-4.2394738976719144E-2</v>
+      </c>
+      <c r="K23">
         <f t="shared" si="4"/>
-        <v>-4.2394738976719144E-2</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="L23">
@@ -2554,15 +3522,15 @@
         <v>22619057.440000001</v>
       </c>
       <c r="N23">
+        <f t="shared" si="5"/>
+        <v>-601242.55999999866</v>
+      </c>
+      <c r="O23" s="5">
         <f t="shared" si="6"/>
-        <v>-601242.55999999866</v>
-      </c>
-      <c r="O23" s="5">
+        <v>-2.5892971236375011E-2</v>
+      </c>
+      <c r="P23">
         <f t="shared" si="7"/>
-        <v>-2.5892971236375011E-2</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="8"/>
         <v>26</v>
       </c>
     </row>
@@ -2585,7 +3553,7 @@
         <v>-1.3334943305713101E-2</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>31</v>
       </c>
       <c r="G24">
@@ -2595,15 +3563,15 @@
         <v>1067214.42</v>
       </c>
       <c r="I24">
+        <f t="shared" si="2"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="J24" s="5">
         <f t="shared" si="3"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="J24" s="5">
+        <v>-4.087856565111897E-2</v>
+      </c>
+      <c r="K24">
         <f t="shared" si="4"/>
-        <v>-4.087856565111897E-2</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="5"/>
         <v>28</v>
       </c>
       <c r="L24">
@@ -2613,15 +3581,15 @@
         <v>1112527.1200000001</v>
       </c>
       <c r="N24">
+        <f t="shared" si="5"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="O24" s="5">
         <f t="shared" si="6"/>
-        <v>-72.879999999888241</v>
-      </c>
-      <c r="O24" s="5">
+        <v>-6.5504224339284781E-5</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="7"/>
-        <v>-6.5504224339284781E-5</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="8"/>
         <v>41</v>
       </c>
     </row>
@@ -2644,7 +3612,7 @@
         <v>-1.0226130964676661E-2</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
       <c r="G25">
@@ -2654,15 +3622,15 @@
         <v>497194.20999999897</v>
       </c>
       <c r="I25">
+        <f t="shared" si="2"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="J25" s="5">
         <f t="shared" si="3"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="J25" s="5">
+        <v>-1.5846773555029746E-2</v>
+      </c>
+      <c r="K25">
         <f t="shared" si="4"/>
-        <v>-1.5846773555029746E-2</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="5"/>
         <v>37</v>
       </c>
       <c r="L25">
@@ -2672,15 +3640,15 @@
         <v>494775.1</v>
       </c>
       <c r="N25">
+        <f t="shared" si="5"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="O25" s="5">
         <f t="shared" si="6"/>
-        <v>-1724.9000000000233</v>
-      </c>
-      <c r="O25" s="5">
+        <v>-3.4741188318228064E-3</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="7"/>
-        <v>-3.4741188318228064E-3</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="8"/>
         <v>35</v>
       </c>
     </row>
@@ -2703,7 +3671,7 @@
         <v>-8.5306091660634673E-2</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="G26">
@@ -2713,15 +3681,15 @@
         <v>5122329.02999999</v>
       </c>
       <c r="I26">
+        <f t="shared" si="2"/>
+        <v>-319870.97000000998</v>
+      </c>
+      <c r="J26" s="5">
         <f t="shared" si="3"/>
-        <v>-319870.97000000998</v>
-      </c>
-      <c r="J26" s="5">
+        <v>-5.8776040939327839E-2</v>
+      </c>
+      <c r="K26">
         <f t="shared" si="4"/>
-        <v>-5.8776040939327839E-2</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="L26">
@@ -2731,15 +3699,15 @@
         <v>5117235.21</v>
       </c>
       <c r="N26">
+        <f t="shared" si="5"/>
+        <v>-313464.79000000004</v>
+      </c>
+      <c r="O26" s="5">
         <f t="shared" si="6"/>
-        <v>-313464.79000000004</v>
-      </c>
-      <c r="O26" s="5">
+        <v>-5.7720881286022069E-2</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="7"/>
-        <v>-5.7720881286022069E-2</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="8"/>
         <v>13</v>
       </c>
     </row>
@@ -2762,7 +3730,7 @@
         <v/>
       </c>
       <c r="F27" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G27">
@@ -2772,15 +3740,15 @@
         <v>0</v>
       </c>
       <c r="I27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J27" s="5" t="str">
+        <v/>
+      </c>
+      <c r="K27" t="e">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K27" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="L27">
@@ -2790,15 +3758,15 @@
         <v>0</v>
       </c>
       <c r="N27">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="5" t="str">
+        <v/>
+      </c>
+      <c r="P27" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P27" t="e">
-        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2821,7 +3789,7 @@
         <v>-9.5782760864849215E-2</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3</v>
       </c>
       <c r="G28">
@@ -2831,15 +3799,15 @@
         <v>1281335.23</v>
       </c>
       <c r="I28">
+        <f t="shared" si="2"/>
+        <v>-264364.77</v>
+      </c>
+      <c r="J28" s="5">
         <f t="shared" si="3"/>
-        <v>-264364.77</v>
-      </c>
-      <c r="J28" s="5">
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="K28">
         <f t="shared" si="4"/>
-        <v>-0.17103239309050916</v>
-      </c>
-      <c r="K28">
-        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="L28">
@@ -2849,15 +3817,15 @@
         <v>1393285.06</v>
       </c>
       <c r="N28">
+        <f t="shared" si="5"/>
+        <v>-132614.93999999994</v>
+      </c>
+      <c r="O28" s="5">
         <f t="shared" si="6"/>
-        <v>-132614.93999999994</v>
-      </c>
-      <c r="O28" s="5">
+        <v>-8.6909325643882263E-2</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="7"/>
-        <v>-8.6909325643882263E-2</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="8"/>
         <v>7</v>
       </c>
     </row>
@@ -2880,7 +3848,7 @@
         <v>-1.4800253727847622E-2</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
       <c r="G29">
@@ -2890,15 +3858,15 @@
         <v>2665264.4399999902</v>
       </c>
       <c r="I29">
+        <f t="shared" si="2"/>
+        <v>-114235.56000000983</v>
+      </c>
+      <c r="J29" s="5">
         <f t="shared" si="3"/>
-        <v>-114235.56000000983</v>
-      </c>
-      <c r="J29" s="5">
+        <v>-4.1099320021590155E-2</v>
+      </c>
+      <c r="K29">
         <f t="shared" si="4"/>
-        <v>-4.1099320021590155E-2</v>
-      </c>
-      <c r="K29">
-        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="L29">
@@ -2908,15 +3876,15 @@
         <v>2889864.67</v>
       </c>
       <c r="N29">
+        <f t="shared" si="5"/>
+        <v>-35.330000000074506</v>
+      </c>
+      <c r="O29" s="5">
         <f t="shared" si="6"/>
-        <v>-35.330000000074506</v>
-      </c>
-      <c r="O29" s="5">
+        <v>-1.2225336516860273E-5</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="7"/>
-        <v>-1.2225336516860273E-5</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="8"/>
         <v>44</v>
       </c>
     </row>
@@ -2939,7 +3907,7 @@
         <v>-8.3831374359143746E-3</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
       <c r="G30">
@@ -2949,15 +3917,15 @@
         <v>12685514.279999901</v>
       </c>
       <c r="I30">
+        <f t="shared" si="2"/>
+        <v>-50385.720000099391</v>
+      </c>
+      <c r="J30" s="5">
         <f t="shared" si="3"/>
-        <v>-50385.720000099391</v>
-      </c>
-      <c r="J30" s="5">
+        <v>-3.9561962641116366E-3</v>
+      </c>
+      <c r="K30">
         <f t="shared" si="4"/>
-        <v>-3.9561962641116366E-3</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="5"/>
         <v>42</v>
       </c>
       <c r="L30">
@@ -2967,15 +3935,15 @@
         <v>12826009.609999999</v>
       </c>
       <c r="N30">
+        <f t="shared" si="5"/>
+        <v>-35290.390000000596</v>
+      </c>
+      <c r="O30" s="5">
         <f t="shared" si="6"/>
-        <v>-35290.390000000596</v>
-      </c>
-      <c r="O30" s="5">
+        <v>-2.7439209100169185E-3</v>
+      </c>
+      <c r="P30">
         <f t="shared" si="7"/>
-        <v>-2.7439209100169185E-3</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="8"/>
         <v>36</v>
       </c>
     </row>
@@ -2998,7 +3966,7 @@
         <v>-1.4030533529678329E-2</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
       <c r="G31">
@@ -3008,15 +3976,15 @@
         <v>1762676.85</v>
       </c>
       <c r="I31">
+        <f t="shared" si="2"/>
+        <v>-60623.149999999907</v>
+      </c>
+      <c r="J31" s="5">
         <f t="shared" si="3"/>
-        <v>-60623.149999999907</v>
-      </c>
-      <c r="J31" s="5">
+        <v>-3.3249136181648611E-2</v>
+      </c>
+      <c r="K31">
         <f t="shared" si="4"/>
-        <v>-3.3249136181648611E-2</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="L31">
@@ -3026,15 +3994,15 @@
         <v>1801391.34</v>
       </c>
       <c r="N31">
+        <f t="shared" si="5"/>
+        <v>-69308.659999999916</v>
+      </c>
+      <c r="O31" s="5">
         <f t="shared" si="6"/>
-        <v>-69308.659999999916</v>
-      </c>
-      <c r="O31" s="5">
+        <v>-3.7049585716576634E-2</v>
+      </c>
+      <c r="P31">
         <f t="shared" si="7"/>
-        <v>-3.7049585716576634E-2</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="8"/>
         <v>20</v>
       </c>
     </row>
@@ -3057,7 +4025,7 @@
         <v>-1.2294942827617691E-2</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
       <c r="G32">
@@ -3067,15 +4035,15 @@
         <v>6084985.4699999997</v>
       </c>
       <c r="I32">
+        <f t="shared" si="2"/>
+        <v>-110514.53000000026</v>
+      </c>
+      <c r="J32" s="5">
         <f t="shared" si="3"/>
-        <v>-110514.53000000026</v>
-      </c>
-      <c r="J32" s="5">
+        <v>-1.7837871035428981E-2</v>
+      </c>
+      <c r="K32">
         <f t="shared" si="4"/>
-        <v>-1.7837871035428981E-2</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="5"/>
         <v>35</v>
       </c>
       <c r="L32">
@@ -3085,15 +4053,15 @@
         <v>5987572.0199999996</v>
       </c>
       <c r="N32">
+        <f t="shared" si="5"/>
+        <v>-169827.98000000045</v>
+      </c>
+      <c r="O32" s="5">
         <f t="shared" si="6"/>
-        <v>-169827.98000000045</v>
-      </c>
-      <c r="O32" s="5">
+        <v>-2.7581118653977402E-2</v>
+      </c>
+      <c r="P32">
         <f t="shared" si="7"/>
-        <v>-2.7581118653977402E-2</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="8"/>
         <v>23</v>
       </c>
     </row>
@@ -3116,7 +4084,7 @@
         <v>-7.9969930789269058E-3</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
       <c r="G33">
@@ -3126,15 +4094,15 @@
         <v>977068513.48000002</v>
       </c>
       <c r="I33">
+        <f t="shared" si="2"/>
+        <v>-2602486.5199999809</v>
+      </c>
+      <c r="J33" s="5">
         <f t="shared" si="3"/>
-        <v>-2602486.5199999809</v>
-      </c>
-      <c r="J33" s="5">
+        <v>-2.6564903115433454E-3</v>
+      </c>
+      <c r="K33">
         <f t="shared" si="4"/>
-        <v>-2.6564903115433454E-3</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="L33">
@@ -3144,15 +4112,15 @@
         <v>984116289.40999901</v>
       </c>
       <c r="N33">
+        <f t="shared" si="5"/>
+        <v>-5456610.5900000334</v>
+      </c>
+      <c r="O33" s="5">
         <f t="shared" si="6"/>
-        <v>-5456610.5900000334</v>
-      </c>
-      <c r="O33" s="5">
+        <v>-5.5141067323084929E-3</v>
+      </c>
+      <c r="P33">
         <f t="shared" si="7"/>
-        <v>-5.5141067323084929E-3</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="8"/>
         <v>34</v>
       </c>
     </row>
@@ -3175,7 +4143,7 @@
         <v>-1.8939149738619768E-2</v>
       </c>
       <c r="F34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="G34">
@@ -3185,15 +4153,15 @@
         <v>4137588.7699999898</v>
       </c>
       <c r="I34">
+        <f t="shared" si="2"/>
+        <v>-213011.23000001023</v>
+      </c>
+      <c r="J34" s="5">
         <f t="shared" si="3"/>
-        <v>-213011.23000001023</v>
-      </c>
-      <c r="J34" s="5">
+        <v>-4.8961345561534093E-2</v>
+      </c>
+      <c r="K34">
         <f t="shared" si="4"/>
-        <v>-4.8961345561534093E-2</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="L34">
@@ -3203,15 +4171,15 @@
         <v>4229801.51</v>
       </c>
       <c r="N34">
+        <f t="shared" si="5"/>
+        <v>-115798.49000000022</v>
+      </c>
+      <c r="O34" s="5">
         <f t="shared" si="6"/>
-        <v>-115798.49000000022</v>
-      </c>
-      <c r="O34" s="5">
+        <v>-2.6647296115611244E-2</v>
+      </c>
+      <c r="P34">
         <f t="shared" si="7"/>
-        <v>-2.6647296115611244E-2</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="8"/>
         <v>24</v>
       </c>
     </row>
@@ -3234,7 +4202,7 @@
         <v/>
       </c>
       <c r="F35" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G35">
@@ -3244,15 +4212,15 @@
         <v>0</v>
       </c>
       <c r="I35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="5" t="str">
+        <v/>
+      </c>
+      <c r="K35" t="e">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K35" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="L35">
@@ -3262,15 +4230,15 @@
         <v>0</v>
       </c>
       <c r="N35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="5" t="str">
+        <v/>
+      </c>
+      <c r="P35" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P35" t="e">
-        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -3293,7 +4261,7 @@
         <v>-7.8647857679780775E-2</v>
       </c>
       <c r="F36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="G36">
@@ -3303,15 +4271,15 @@
         <v>740966.94999999902</v>
       </c>
       <c r="I36">
+        <f t="shared" si="2"/>
+        <v>-157733.05000000098</v>
+      </c>
+      <c r="J36" s="5">
         <f t="shared" si="3"/>
-        <v>-157733.05000000098</v>
-      </c>
-      <c r="J36" s="5">
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="K36">
         <f t="shared" si="4"/>
-        <v>-0.17551246244575608</v>
-      </c>
-      <c r="K36">
-        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="L36">
@@ -3321,15 +4289,15 @@
         <v>777215.28999999899</v>
       </c>
       <c r="N36">
+        <f t="shared" si="5"/>
+        <v>-101084.71000000101</v>
+      </c>
+      <c r="O36" s="5">
         <f t="shared" si="6"/>
-        <v>-101084.71000000101</v>
-      </c>
-      <c r="O36" s="5">
+        <v>-0.11509132414892521</v>
+      </c>
+      <c r="P36">
         <f t="shared" si="7"/>
-        <v>-0.11509132414892521</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="8"/>
         <v>5</v>
       </c>
     </row>
@@ -3352,7 +4320,7 @@
         <v>-3.9444515758219188E-2</v>
       </c>
       <c r="F37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="G37">
@@ -3362,15 +4330,15 @@
         <v>2118943.21</v>
       </c>
       <c r="I37">
+        <f t="shared" si="2"/>
+        <v>-110256.79000000004</v>
+      </c>
+      <c r="J37" s="5">
         <f t="shared" si="3"/>
-        <v>-110256.79000000004</v>
-      </c>
-      <c r="J37" s="5">
+        <v>-4.9460250314014013E-2</v>
+      </c>
+      <c r="K37">
         <f t="shared" si="4"/>
-        <v>-4.9460250314014013E-2</v>
-      </c>
-      <c r="K37">
-        <f t="shared" si="5"/>
         <v>20</v>
       </c>
       <c r="L37">
@@ -3380,15 +4348,15 @@
         <v>2108718.34</v>
       </c>
       <c r="N37">
+        <f t="shared" si="5"/>
+        <v>-188181.66000000015</v>
+      </c>
+      <c r="O37" s="5">
         <f t="shared" si="6"/>
-        <v>-188181.66000000015</v>
-      </c>
-      <c r="O37" s="5">
+        <v>-8.1928538464887526E-2</v>
+      </c>
+      <c r="P37">
         <f t="shared" si="7"/>
-        <v>-8.1928538464887526E-2</v>
-      </c>
-      <c r="P37">
-        <f t="shared" si="8"/>
         <v>8</v>
       </c>
     </row>
@@ -3411,7 +4379,7 @@
         <v>-1.9443680579913542E-2</v>
       </c>
       <c r="F38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
       <c r="G38">
@@ -3421,15 +4389,15 @@
         <v>753451.96</v>
       </c>
       <c r="I38">
+        <f t="shared" si="2"/>
+        <v>-39348.040000000037</v>
+      </c>
+      <c r="J38" s="5">
         <f t="shared" si="3"/>
-        <v>-39348.040000000037</v>
-      </c>
-      <c r="J38" s="5">
+        <v>-4.9631735620585316E-2</v>
+      </c>
+      <c r="K38">
         <f t="shared" si="4"/>
-        <v>-4.9631735620585316E-2</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="L38">
@@ -3439,15 +4407,15 @@
         <v>777663.26</v>
       </c>
       <c r="N38">
+        <f t="shared" si="5"/>
+        <v>-136.73999999999069</v>
+      </c>
+      <c r="O38" s="5">
         <f t="shared" si="6"/>
-        <v>-136.73999999999069</v>
-      </c>
-      <c r="O38" s="5">
+        <v>-1.7580354847003174E-4</v>
+      </c>
+      <c r="P38">
         <f t="shared" si="7"/>
-        <v>-1.7580354847003174E-4</v>
-      </c>
-      <c r="P38">
-        <f t="shared" si="8"/>
         <v>40</v>
       </c>
     </row>
@@ -3470,7 +4438,7 @@
         <v>-8.008952370177623E-2</v>
       </c>
       <c r="F39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>8</v>
       </c>
       <c r="G39">
@@ -3480,15 +4448,15 @@
         <v>1114242.27999999</v>
       </c>
       <c r="I39">
+        <f t="shared" si="2"/>
+        <v>-180157.72000000998</v>
+      </c>
+      <c r="J39" s="5">
         <f t="shared" si="3"/>
-        <v>-180157.72000000998</v>
-      </c>
-      <c r="J39" s="5">
+        <v>-0.13918241656366656</v>
+      </c>
+      <c r="K39">
         <f t="shared" si="4"/>
-        <v>-0.13918241656366656</v>
-      </c>
-      <c r="K39">
-        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="L39">
@@ -3498,15 +4466,15 @@
         <v>1680463.8699999901</v>
       </c>
       <c r="N39">
+        <f t="shared" si="5"/>
+        <v>-79036.1300000099</v>
+      </c>
+      <c r="O39" s="5">
         <f t="shared" si="6"/>
-        <v>-79036.1300000099</v>
-      </c>
-      <c r="O39" s="5">
+        <v>-4.4919653310605226E-2</v>
+      </c>
+      <c r="P39">
         <f t="shared" si="7"/>
-        <v>-4.4919653310605226E-2</v>
-      </c>
-      <c r="P39">
-        <f t="shared" si="8"/>
         <v>17</v>
       </c>
     </row>
@@ -3529,7 +4497,7 @@
         <v>-2.1279773539092578E-2</v>
       </c>
       <c r="F40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="G40">
@@ -3539,15 +4507,15 @@
         <v>38095240.189999901</v>
       </c>
       <c r="I40">
+        <f t="shared" si="2"/>
+        <v>-1869659.8100000992</v>
+      </c>
+      <c r="J40" s="5">
         <f t="shared" si="3"/>
-        <v>-1869659.8100000992</v>
-      </c>
-      <c r="J40" s="5">
+        <v>-4.6782546934937892E-2</v>
+      </c>
+      <c r="K40">
         <f t="shared" si="4"/>
-        <v>-4.6782546934937892E-2</v>
-      </c>
-      <c r="K40">
-        <f t="shared" si="5"/>
         <v>22</v>
       </c>
       <c r="L40">
@@ -3557,15 +4525,15 @@
         <v>39606263.709999897</v>
       </c>
       <c r="N40">
+        <f t="shared" si="5"/>
+        <v>-610436.29000010341</v>
+      </c>
+      <c r="O40" s="5">
         <f t="shared" si="6"/>
-        <v>-610436.29000010341</v>
-      </c>
-      <c r="O40" s="5">
+        <v>-1.5178676768608648E-2</v>
+      </c>
+      <c r="P40">
         <f t="shared" si="7"/>
-        <v>-1.5178676768608648E-2</v>
-      </c>
-      <c r="P40">
-        <f t="shared" si="8"/>
         <v>31</v>
       </c>
     </row>
@@ -3588,7 +4556,7 @@
         <v>-4.0110550149132493E-2</v>
       </c>
       <c r="F41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="G41">
@@ -3598,15 +4566,15 @@
         <v>4956043.6699999897</v>
       </c>
       <c r="I41">
+        <f t="shared" si="2"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="J41" s="5">
         <f t="shared" si="3"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="J41" s="5">
+        <v>-2.6221894095689226E-2</v>
+      </c>
+      <c r="K41">
         <f t="shared" si="4"/>
-        <v>-2.6221894095689226E-2</v>
-      </c>
-      <c r="K41">
-        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="L41">
@@ -3616,15 +4584,15 @@
         <v>4717822.6500000004</v>
       </c>
       <c r="N41">
+        <f t="shared" si="5"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="O41" s="5">
         <f t="shared" si="6"/>
-        <v>-82077.349999999627</v>
-      </c>
-      <c r="O41" s="5">
+        <v>-1.7099804162586642E-2</v>
+      </c>
+      <c r="P41">
         <f t="shared" si="7"/>
-        <v>-1.7099804162586642E-2</v>
-      </c>
-      <c r="P41">
-        <f t="shared" si="8"/>
         <v>30</v>
       </c>
     </row>
@@ -3647,7 +4615,7 @@
         <v>-2.2070943135841053E-4</v>
       </c>
       <c r="F42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
       <c r="G42">
@@ -3657,15 +4625,15 @@
         <v>196755033.31</v>
       </c>
       <c r="I42">
+        <f t="shared" si="2"/>
+        <v>-2375266.6899999976</v>
+      </c>
+      <c r="J42" s="5">
         <f t="shared" si="3"/>
-        <v>-2375266.6899999976</v>
-      </c>
-      <c r="J42" s="5">
+        <v>-1.1928203241796942E-2</v>
+      </c>
+      <c r="K42">
         <f t="shared" si="4"/>
-        <v>-1.1928203241796942E-2</v>
-      </c>
-      <c r="K42">
-        <f t="shared" si="5"/>
         <v>39</v>
       </c>
       <c r="L42">
@@ -3675,15 +4643,15 @@
         <v>199954563.74999899</v>
       </c>
       <c r="N42">
+        <f t="shared" si="5"/>
+        <v>-36.250001013278961</v>
+      </c>
+      <c r="O42" s="5">
         <f t="shared" si="6"/>
-        <v>-36.250001013278961</v>
-      </c>
-      <c r="O42" s="5">
+        <v>-1.8129115815929696E-7</v>
+      </c>
+      <c r="P42">
         <f t="shared" si="7"/>
-        <v>-1.8129115815929696E-7</v>
-      </c>
-      <c r="P42">
-        <f t="shared" si="8"/>
         <v>47</v>
       </c>
     </row>
@@ -3706,7 +4674,7 @@
         <v>-2.0497353541313264E-2</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="G43">
@@ -3716,15 +4684,15 @@
         <v>8171472.0199999996</v>
       </c>
       <c r="I43">
+        <f t="shared" si="2"/>
+        <v>-389327.98000000045</v>
+      </c>
+      <c r="J43" s="5">
         <f t="shared" si="3"/>
-        <v>-389327.98000000045</v>
-      </c>
-      <c r="J43" s="5">
+        <v>-4.5477990374731388E-2</v>
+      </c>
+      <c r="K43">
         <f t="shared" si="4"/>
-        <v>-4.5477990374731388E-2</v>
-      </c>
-      <c r="K43">
-        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="L43">
@@ -3734,15 +4702,15 @@
         <v>8150982.5699999901</v>
       </c>
       <c r="N43">
+        <f t="shared" si="5"/>
+        <v>-346517.43000000995</v>
+      </c>
+      <c r="O43" s="5">
         <f t="shared" si="6"/>
-        <v>-346517.43000000995</v>
-      </c>
-      <c r="O43" s="5">
+        <v>-4.0778750220654303E-2</v>
+      </c>
+      <c r="P43">
         <f t="shared" si="7"/>
-        <v>-4.0778750220654303E-2</v>
-      </c>
-      <c r="P43">
-        <f t="shared" si="8"/>
         <v>18</v>
       </c>
     </row>
@@ -3765,7 +4733,7 @@
         <v>-9.7760750186150751E-3</v>
       </c>
       <c r="F44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>39</v>
       </c>
       <c r="G44">
@@ -3775,15 +4743,15 @@
         <v>30793711.48</v>
       </c>
       <c r="I44">
+        <f t="shared" si="2"/>
+        <v>-246988.51999999955</v>
+      </c>
+      <c r="J44" s="5">
         <f t="shared" si="3"/>
-        <v>-246988.51999999955</v>
-      </c>
-      <c r="J44" s="5">
+        <v>-7.9569249404813532E-3</v>
+      </c>
+      <c r="K44">
         <f t="shared" si="4"/>
-        <v>-7.9569249404813532E-3</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="5"/>
         <v>41</v>
       </c>
       <c r="L44">
@@ -3793,15 +4761,15 @@
         <v>31282141.25</v>
       </c>
       <c r="N44">
+        <f t="shared" si="5"/>
+        <v>-58.75</v>
+      </c>
+      <c r="O44" s="5">
         <f t="shared" si="6"/>
-        <v>-58.75</v>
-      </c>
-      <c r="O44" s="5">
+        <v>-1.8780648419868168E-6</v>
+      </c>
+      <c r="P44">
         <f t="shared" si="7"/>
-        <v>-1.8780648419868168E-6</v>
-      </c>
-      <c r="P44">
-        <f t="shared" si="8"/>
         <v>45</v>
       </c>
     </row>
@@ -3824,7 +4792,7 @@
         <v>-1.287514194887851E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
       <c r="G45">
@@ -3834,15 +4802,15 @@
         <v>54594953.959999897</v>
       </c>
       <c r="I45">
+        <f t="shared" si="2"/>
+        <v>-2197246.0400001034</v>
+      </c>
+      <c r="J45" s="5">
         <f t="shared" si="3"/>
-        <v>-2197246.0400001034</v>
-      </c>
-      <c r="J45" s="5">
+        <v>-3.8689222111488959E-2</v>
+      </c>
+      <c r="K45">
         <f t="shared" si="4"/>
-        <v>-3.8689222111488959E-2</v>
-      </c>
-      <c r="K45">
-        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="L45">
@@ -3852,15 +4820,15 @@
         <v>55386549.6599999</v>
       </c>
       <c r="N45">
+        <f t="shared" si="5"/>
+        <v>-640550.34000010043</v>
+      </c>
+      <c r="O45" s="5">
         <f t="shared" si="6"/>
-        <v>-640550.34000010043</v>
-      </c>
-      <c r="O45" s="5">
+        <v>-1.1432866237947358E-2</v>
+      </c>
+      <c r="P45">
         <f t="shared" si="7"/>
-        <v>-1.1432866237947358E-2</v>
-      </c>
-      <c r="P45">
-        <f t="shared" si="8"/>
         <v>32</v>
       </c>
     </row>
@@ -3883,7 +4851,7 @@
         <v>-3.0010420686993711E-3</v>
       </c>
       <c r="F46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>43</v>
       </c>
       <c r="G46">
@@ -3893,15 +4861,15 @@
         <v>257402.90999999901</v>
       </c>
       <c r="I46">
+        <f t="shared" si="2"/>
+        <v>-8597.090000000986</v>
+      </c>
+      <c r="J46" s="5">
         <f t="shared" si="3"/>
-        <v>-8597.090000000986</v>
-      </c>
-      <c r="J46" s="5">
+        <v>-3.2319887218048821E-2</v>
+      </c>
+      <c r="K46">
         <f t="shared" si="4"/>
-        <v>-3.2319887218048821E-2</v>
-      </c>
-      <c r="K46">
-        <f t="shared" si="5"/>
         <v>33</v>
       </c>
       <c r="L46">
@@ -3911,15 +4879,15 @@
         <v>254753.15999999901</v>
       </c>
       <c r="N46">
+        <f t="shared" si="5"/>
+        <v>-12346.840000000986</v>
+      </c>
+      <c r="O46" s="5">
         <f t="shared" si="6"/>
-        <v>-12346.840000000986</v>
-      </c>
-      <c r="O46" s="5">
+        <v>-4.6225533508053113E-2</v>
+      </c>
+      <c r="P46">
         <f t="shared" si="7"/>
-        <v>-4.6225533508053113E-2</v>
-      </c>
-      <c r="P46">
-        <f t="shared" si="8"/>
         <v>16</v>
       </c>
     </row>
@@ -3942,7 +4910,7 @@
         <v>-1.7435939690898361E-4</v>
       </c>
       <c r="F47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
       <c r="G47">
@@ -3952,15 +4920,15 @@
         <v>73442541.659999996</v>
       </c>
       <c r="I47">
+        <f t="shared" si="2"/>
+        <v>-24458.340000003576</v>
+      </c>
+      <c r="J47" s="5">
         <f t="shared" si="3"/>
-        <v>-24458.340000003576</v>
-      </c>
-      <c r="J47" s="5">
+        <v>-3.3291600310348285E-4</v>
+      </c>
+      <c r="K47">
         <f t="shared" si="4"/>
-        <v>-3.3291600310348285E-4</v>
-      </c>
-      <c r="K47">
-        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="L47">
@@ -3970,15 +4938,15 @@
         <v>75050829.179999903</v>
       </c>
       <c r="N47">
+        <f t="shared" si="5"/>
+        <v>-21970.820000097156</v>
+      </c>
+      <c r="O47" s="5">
         <f t="shared" si="6"/>
-        <v>-21970.820000097156</v>
-      </c>
-      <c r="O47" s="5">
+        <v>-2.9266019117572752E-4</v>
+      </c>
+      <c r="P47">
         <f t="shared" si="7"/>
-        <v>-2.9266019117572752E-4</v>
-      </c>
-      <c r="P47">
-        <f t="shared" si="8"/>
         <v>38</v>
       </c>
     </row>
@@ -4001,7 +4969,7 @@
         <v>-3.1133192323107857E-2</v>
       </c>
       <c r="F48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="G48">
@@ -4011,15 +4979,15 @@
         <v>6922072.5599999996</v>
       </c>
       <c r="I48">
+        <f t="shared" si="2"/>
+        <v>-292627.44000000041</v>
+      </c>
+      <c r="J48" s="5">
         <f t="shared" si="3"/>
-        <v>-292627.44000000041</v>
-      </c>
-      <c r="J48" s="5">
+        <v>-4.0559890224125802E-2</v>
+      </c>
+      <c r="K48">
         <f t="shared" si="4"/>
-        <v>-4.0559890224125802E-2</v>
-      </c>
-      <c r="K48">
-        <f t="shared" si="5"/>
         <v>29</v>
       </c>
       <c r="L48">
@@ -4029,15 +4997,15 @@
         <v>6882350.23999999</v>
       </c>
       <c r="N48">
+        <f t="shared" si="5"/>
+        <v>-407449.76000001002</v>
+      </c>
+      <c r="O48" s="5">
         <f t="shared" si="6"/>
-        <v>-407449.76000001002</v>
-      </c>
-      <c r="O48" s="5">
+        <v>-5.5893132870587676E-2</v>
+      </c>
+      <c r="P48">
         <f t="shared" si="7"/>
-        <v>-5.5893132870587676E-2</v>
-      </c>
-      <c r="P48">
-        <f t="shared" si="8"/>
         <v>15</v>
       </c>
     </row>
@@ -4060,7 +5028,7 @@
         <v>-1.8444360086767971E-2</v>
       </c>
       <c r="F49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
       <c r="G49">
@@ -4070,15 +5038,15 @@
         <v>95466.880000000005</v>
       </c>
       <c r="I49">
+        <f t="shared" si="2"/>
+        <v>-7133.1199999999953</v>
+      </c>
+      <c r="J49" s="5">
         <f t="shared" si="3"/>
-        <v>-7133.1199999999953</v>
-      </c>
-      <c r="J49" s="5">
+        <v>-6.9523586744639335E-2</v>
+      </c>
+      <c r="K49">
         <f t="shared" si="4"/>
-        <v>-6.9523586744639335E-2</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="L49">
@@ -4088,15 +5056,15 @@
         <v>0</v>
       </c>
       <c r="N49">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O49" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O49" s="5" t="str">
+        <v/>
+      </c>
+      <c r="P49" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P49" t="e">
-        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -4119,7 +5087,7 @@
         <v/>
       </c>
       <c r="F50" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="G50">
@@ -4129,15 +5097,15 @@
         <v>859100</v>
       </c>
       <c r="I50">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J50" s="5" t="str">
+        <v/>
+      </c>
+      <c r="K50" t="e">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="K50" t="e">
-        <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
       <c r="L50">
@@ -4147,15 +5115,15 @@
         <v>843200</v>
       </c>
       <c r="N50">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="5" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="O50" s="5" t="str">
+        <v/>
+      </c>
+      <c r="P50" t="e">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="P50" t="e">
-        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -4178,7 +5146,7 @@
         <v>-1.2785255822058129E-2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
       <c r="G51">
@@ -4188,15 +5156,15 @@
         <v>8599059.6199999992</v>
       </c>
       <c r="I51">
+        <f t="shared" si="2"/>
+        <v>-326440.38000000082</v>
+      </c>
+      <c r="J51" s="5">
         <f t="shared" si="3"/>
-        <v>-326440.38000000082</v>
-      </c>
-      <c r="J51" s="5">
+        <v>-3.6573903982970231E-2</v>
+      </c>
+      <c r="K51">
         <f t="shared" si="4"/>
-        <v>-3.6573903982970231E-2</v>
-      </c>
-      <c r="K51">
-        <f t="shared" si="5"/>
         <v>31</v>
       </c>
       <c r="L51">
@@ -4206,15 +5174,15 @@
         <v>8735843.3100000005</v>
       </c>
       <c r="N51">
+        <f t="shared" si="5"/>
+        <v>-98056.689999999478</v>
+      </c>
+      <c r="O51" s="5">
         <f t="shared" si="6"/>
-        <v>-98056.689999999478</v>
-      </c>
-      <c r="O51" s="5">
+        <v>-1.1100045280114048E-2</v>
+      </c>
+      <c r="P51">
         <f t="shared" si="7"/>
-        <v>-1.1100045280114048E-2</v>
-      </c>
-      <c r="P51">
-        <f t="shared" si="8"/>
         <v>33</v>
       </c>
     </row>
@@ -4237,7 +5205,7 @@
         <v>-8.009596083231342E-2</v>
       </c>
       <c r="F52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>7</v>
       </c>
       <c r="G52">
@@ -4247,15 +5215,15 @@
         <v>2204672.88</v>
       </c>
       <c r="I52">
+        <f t="shared" si="2"/>
+        <v>-236027.12000000011</v>
+      </c>
+      <c r="J52" s="5">
         <f t="shared" si="3"/>
-        <v>-236027.12000000011</v>
-      </c>
-      <c r="J52" s="5">
+        <v>-9.6704683082722218E-2</v>
+      </c>
+      <c r="K52">
         <f t="shared" si="4"/>
-        <v>-9.6704683082722218E-2</v>
-      </c>
-      <c r="K52">
-        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="L52">
@@ -4265,15 +5233,15 @@
         <v>2056835.26</v>
       </c>
       <c r="N52">
+        <f t="shared" si="5"/>
+        <v>-264764.74</v>
+      </c>
+      <c r="O52" s="5">
         <f t="shared" si="6"/>
-        <v>-264764.74</v>
-      </c>
-      <c r="O52" s="5">
+        <v>-0.11404408166781529</v>
+      </c>
+      <c r="P52">
         <f t="shared" si="7"/>
-        <v>-0.11404408166781529</v>
-      </c>
-      <c r="P52">
-        <f t="shared" si="8"/>
         <v>6</v>
       </c>
     </row>
@@ -4318,7 +5286,7 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A57,$A$2:$P$52,MATCH(B$55,$A$1:$P$1,0),FALSE)</f>
+        <f>VLOOKUP($A57,$A$2:$P$52,MATCH(B$55,$A$1:$P$1,0),FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
@@ -4335,7 +5303,7 @@
         <v>32</v>
       </c>
       <c r="B58">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A58,$A$2:$P$52,MATCH(B$55,$A$1:$P$1,0),FALSE)</f>
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
@@ -4386,7 +5354,7 @@
         <v>55</v>
       </c>
       <c r="B61">
-        <f t="shared" si="10"/>
+        <f>VLOOKUP($A61,$A$2:$P$52,MATCH(B$55,$A$1:$P$1,0),FALSE)</f>
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
@@ -4550,11 +5518,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f t="shared" ref="C74:D79" si="11">INDEX($B$2:$P$52,MATCH($A74,$A$2:$A$52,0),MATCH(C$73,$B$1:$P$1,0))</f>
+        <f>INDEX($B$2:$P$52,MATCH($A74,$A$2:$A$52,0),MATCH(C$73,$B$1:$P$1,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="C74:D79" si="11">INDEX($B$2:$P$52,MATCH($A74,$A$2:$A$52,0),MATCH(D$73,$B$1:$P$1,0))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4567,7 +5535,7 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" si="11"/>
+        <f>INDEX($B$2:$P$52,MATCH($A75,$A$2:$A$52,0),MATCH(C$73,$B$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
@@ -4667,11 +5635,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B$2:B$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>3130600</v>
+        <v>20862700</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C$2:C$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>3115157.5599999898</v>
+        <v>20036743.4099999</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4680,11 +5648,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G$2:G$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>3652300</v>
+        <v>22683800</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H$2:H$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>3589693.2099999902</v>
+        <v>21722126.219999898</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4693,16 +5661,16 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L$2:L$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>3662400</v>
+        <v>23220300</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(M$2:M$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>3564983.04999999</v>
+        <v>22619057.440000001</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4972,6 +5940,10 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C91:C93 E91:E93 E98:E100 C98:C100 D98:D100 F98:F100 F91:F93 D91:D93" formula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>